<commit_message>
major changes - March 2021
</commit_message>
<xml_diff>
--- a/Scenario_configurator/1_SETS.xlsx
+++ b/Scenario_configurator/1_SETS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riccardo Novo\Documents\GitHub\OSeMOSYS_Pyomo\Scenario_configurator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D3F20E-E120-4832-9F51-FB21B232CD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4644F6B-B36E-43B1-B562-CF5C7BF65312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="1" r:id="rId1"/>
@@ -33,11 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>REGION</t>
   </si>
   <si>
+    <t>PAN</t>
+  </si>
+  <si>
     <t>DAYTYPE</t>
   </si>
   <si>
@@ -66,13 +69,34 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>S1D1T1</t>
+  </si>
+  <si>
+    <t>S1D1T2</t>
+  </si>
+  <si>
+    <t>S1D1T3</t>
+  </si>
+  <si>
+    <t>DIESEL_PP</t>
+  </si>
+  <si>
+    <t>BIOMASS_PP</t>
+  </si>
+  <si>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>ELC_FD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +106,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +154,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -405,11 +444,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Foglio1"/>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,39 +467,238 @@
     <col min="12" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5" s="3">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8" s="3">
+        <v>2026</v>
+      </c>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9" s="3">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="6"/>
+      <c r="K10" s="3">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12" s="3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="3">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15" s="3">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K16" s="3">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="3">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="3">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="3">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="3">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="3">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="3">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="3">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="3">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="3">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="3">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="3">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="3">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="3">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="3">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="3">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="3">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>
@@ -470,4 +708,226 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100EB3ED1DF6074BB428EE94B4D0572869F" ma:contentTypeVersion="8" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="a8abe48695535b20373e3077406790c6">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f009ebc-ad35-4deb-9fb5-d91b0c3f741e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="367691e11e19abcec54310c8436fdd8f" ns2:_="">
+    <xsd:import namespace="3f009ebc-ad35-4deb-9fb5-d91b0c3f741e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3f009ebc-ad35-4deb-9fb5-d91b0c3f741e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB1A9A31-5D83-4297-A387-783B8E03C5B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072DFFFE-43C2-42B3-82C3-56E8561DA815}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3f009ebc-ad35-4deb-9fb5-d91b0c3f741e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{549E9C59-F3A8-4F09-8949-1D9DFEE9C689}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>